<commit_message>
Add case 4 and 5
Push before adding seeds to struct
</commit_message>
<xml_diff>
--- a/Sommerstudenter_timeliste.xlsx
+++ b/Sommerstudenter_timeliste.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vn123\OneDrive\Master\MRST\summer_sintef\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e8351a88428b982e/Master/MRST/summer_sintef/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D8D401-83F7-4C26-BE01-B69150FE2CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{A2D8D401-83F7-4C26-BE01-B69150FE2CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CE9293F-BF08-44D4-9264-8A574A2007E0}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D8EFFAFB-49CB-4648-896C-712D84251768}"/>
   </bookViews>
@@ -906,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C3154B0-9389-4599-8069-8924A759F725}">
   <dimension ref="B3:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:E5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="82" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1213,16 +1213,26 @@
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
+      <c r="F17" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="G17" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="H17" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="I17" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="J17" s="4">
+        <v>7.5</v>
+      </c>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
       <c r="M17" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>37.5</v>
       </c>
     </row>
     <row r="18" spans="2:17" ht="15" thickBot="1">
@@ -1327,16 +1337,26 @@
       <c r="C23" s="14"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
+      <c r="F23" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="G23" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="H23" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="I23" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="J23" s="4">
+        <v>7.5</v>
+      </c>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
       <c r="M23" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>37.5</v>
       </c>
     </row>
     <row r="24" spans="2:17" ht="15" thickBot="1">

</xml_diff>